<commit_message>
Fixed bug in enviornment that didn't keep track of prices accurately. Need to retrain. So far RNN is king over MLP.
</commit_message>
<xml_diff>
--- a/Energy Price_2016.xlsx
+++ b/Energy Price_2016.xlsx
@@ -492,7 +492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -509,7 +509,7 @@
         <f>D2/1000</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -526,7 +526,7 @@
         <f>D3/1000</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -543,7 +543,7 @@
         <f>D4/1000</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -560,7 +560,7 @@
         <f>D5/1000</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
@@ -577,7 +577,7 @@
         <f>D6/1000</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -594,7 +594,7 @@
         <f>D7/1000</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -611,7 +611,7 @@
         <f>D8/1000</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
@@ -628,7 +628,7 @@
         <f>D9/1000</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -645,7 +645,7 @@
         <f>D10/1000</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="6" t="s">
         <v>5</v>
       </c>
@@ -662,7 +662,7 @@
         <f>D11/1000</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="6" t="s">
         <v>5</v>
       </c>

</xml_diff>